<commit_message>
APResolution now retrieved from MovieDatabase.xlsx
</commit_message>
<xml_diff>
--- a/InstallationFiles/MovieDatabase.xlsx
+++ b/InstallationFiles/MovieDatabase.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Hernan\mRNADynamics\InstallationFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Armando\mRNADynamics\InstallationFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17265"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$T$2</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>ExperimentAxis</t>
+  </si>
+  <si>
+    <t>APResolution</t>
   </si>
 </sst>
 </file>
@@ -691,31 +694,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.6328125" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,55 +736,58 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="S2" s="4"/>
+      <c r="L2" s="6"/>
+      <c r="T2" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R2"/>
+  <autoFilter ref="A1:S2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
@@ -797,7 +804,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -814,7 +821,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>